<commit_message>
10 first photos labelled.
</commit_message>
<xml_diff>
--- a/labellisation.xlsx
+++ b/labellisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nizon\Documents\Perso\Cours\Cours 4A\The AI Lifecycle\App-For-People-With-Restricted-Diet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BCBA04-83C5-449E-A85D-E20428395455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A771E057-2346-418B-9643-BEB887757101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>barley</t>
   </si>
   <si>
-    <t>Select also nuts when there is at least peanuts, almonds or hazelnuts. If whey, put it with milk.</t>
-  </si>
-  <si>
     <t>001.png</t>
   </si>
   <si>
@@ -744,6 +741,9 @@
   </si>
   <si>
     <t>222.png</t>
+  </si>
+  <si>
+    <t>Select also nuts when there is at least peanuts, almonds or hazelnuts. If whey, put it with milk. Also consider "traces of".</t>
   </si>
 </sst>
 </file>
@@ -1098,15 +1098,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
-      <selection activeCell="N222" sqref="N222"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="3" t="s">
-        <v>13</v>
+        <v>235</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1165,177 +1165,417 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1352,7 +1592,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1369,7 +1609,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1386,7 +1626,7 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1403,7 +1643,7 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1420,7 +1660,7 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1437,7 +1677,7 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1454,7 +1694,7 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1471,7 +1711,7 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1488,7 +1728,7 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1505,7 +1745,7 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1522,7 +1762,7 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1539,7 +1779,7 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1556,7 +1796,7 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1573,7 +1813,7 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1590,7 +1830,7 @@
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1607,7 +1847,7 @@
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1624,7 +1864,7 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1641,7 +1881,7 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1658,7 +1898,7 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1675,7 +1915,7 @@
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1692,7 +1932,7 @@
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1709,7 +1949,7 @@
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1726,7 +1966,7 @@
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1743,7 +1983,7 @@
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1760,7 +2000,7 @@
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1777,7 +2017,7 @@
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1794,7 +2034,7 @@
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1811,7 +2051,7 @@
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1828,7 +2068,7 @@
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1845,7 +2085,7 @@
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1862,7 +2102,7 @@
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1879,7 +2119,7 @@
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1896,7 +2136,7 @@
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1913,7 +2153,7 @@
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1930,7 +2170,7 @@
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1947,7 +2187,7 @@
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1964,7 +2204,7 @@
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1981,7 +2221,7 @@
     </row>
     <row r="52" spans="1:13">
       <c r="A52" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1998,7 +2238,7 @@
     </row>
     <row r="53" spans="1:13">
       <c r="A53" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2015,7 +2255,7 @@
     </row>
     <row r="54" spans="1:13">
       <c r="A54" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2032,7 +2272,7 @@
     </row>
     <row r="55" spans="1:13">
       <c r="A55" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2049,7 +2289,7 @@
     </row>
     <row r="56" spans="1:13">
       <c r="A56" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2066,7 +2306,7 @@
     </row>
     <row r="57" spans="1:13">
       <c r="A57" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2083,7 +2323,7 @@
     </row>
     <row r="58" spans="1:13">
       <c r="A58" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2100,7 +2340,7 @@
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2117,7 +2357,7 @@
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2134,7 +2374,7 @@
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2151,7 +2391,7 @@
     </row>
     <row r="62" spans="1:13">
       <c r="A62" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2168,7 +2408,7 @@
     </row>
     <row r="63" spans="1:13">
       <c r="A63" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2185,7 +2425,7 @@
     </row>
     <row r="64" spans="1:13">
       <c r="A64" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2202,7 +2442,7 @@
     </row>
     <row r="65" spans="1:13">
       <c r="A65" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2219,7 +2459,7 @@
     </row>
     <row r="66" spans="1:13">
       <c r="A66" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2236,7 +2476,7 @@
     </row>
     <row r="67" spans="1:13">
       <c r="A67" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2253,7 +2493,7 @@
     </row>
     <row r="68" spans="1:13">
       <c r="A68" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2270,7 +2510,7 @@
     </row>
     <row r="69" spans="1:13">
       <c r="A69" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2287,7 +2527,7 @@
     </row>
     <row r="70" spans="1:13">
       <c r="A70" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2304,7 +2544,7 @@
     </row>
     <row r="71" spans="1:13">
       <c r="A71" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2321,7 +2561,7 @@
     </row>
     <row r="72" spans="1:13">
       <c r="A72" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2338,7 +2578,7 @@
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2355,7 +2595,7 @@
     </row>
     <row r="74" spans="1:13">
       <c r="A74" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2372,7 +2612,7 @@
     </row>
     <row r="75" spans="1:13">
       <c r="A75" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2389,7 +2629,7 @@
     </row>
     <row r="76" spans="1:13">
       <c r="A76" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2406,7 +2646,7 @@
     </row>
     <row r="77" spans="1:13">
       <c r="A77" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2423,7 +2663,7 @@
     </row>
     <row r="78" spans="1:13">
       <c r="A78" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2440,7 +2680,7 @@
     </row>
     <row r="79" spans="1:13">
       <c r="A79" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2457,7 +2697,7 @@
     </row>
     <row r="80" spans="1:13">
       <c r="A80" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2474,7 +2714,7 @@
     </row>
     <row r="81" spans="1:13">
       <c r="A81" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2491,7 +2731,7 @@
     </row>
     <row r="82" spans="1:13">
       <c r="A82" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2508,7 +2748,7 @@
     </row>
     <row r="83" spans="1:13">
       <c r="A83" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2525,7 +2765,7 @@
     </row>
     <row r="84" spans="1:13">
       <c r="A84" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2542,7 +2782,7 @@
     </row>
     <row r="85" spans="1:13">
       <c r="A85" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2559,7 +2799,7 @@
     </row>
     <row r="86" spans="1:13">
       <c r="A86" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2576,7 +2816,7 @@
     </row>
     <row r="87" spans="1:13">
       <c r="A87" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2593,7 +2833,7 @@
     </row>
     <row r="88" spans="1:13">
       <c r="A88" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2610,7 +2850,7 @@
     </row>
     <row r="89" spans="1:13">
       <c r="A89" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2627,7 +2867,7 @@
     </row>
     <row r="90" spans="1:13">
       <c r="A90" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2644,7 +2884,7 @@
     </row>
     <row r="91" spans="1:13">
       <c r="A91" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2661,7 +2901,7 @@
     </row>
     <row r="92" spans="1:13">
       <c r="A92" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2678,7 +2918,7 @@
     </row>
     <row r="93" spans="1:13">
       <c r="A93" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2695,7 +2935,7 @@
     </row>
     <row r="94" spans="1:13">
       <c r="A94" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2712,7 +2952,7 @@
     </row>
     <row r="95" spans="1:13">
       <c r="A95" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2729,7 +2969,7 @@
     </row>
     <row r="96" spans="1:13">
       <c r="A96" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2746,7 +2986,7 @@
     </row>
     <row r="97" spans="1:13">
       <c r="A97" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2763,7 +3003,7 @@
     </row>
     <row r="98" spans="1:13">
       <c r="A98" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2780,7 +3020,7 @@
     </row>
     <row r="99" spans="1:13">
       <c r="A99" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2797,7 +3037,7 @@
     </row>
     <row r="100" spans="1:13">
       <c r="A100" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2814,7 +3054,7 @@
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -2831,7 +3071,7 @@
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -2848,7 +3088,7 @@
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -2865,7 +3105,7 @@
     </row>
     <row r="104" spans="1:13">
       <c r="A104" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -2882,7 +3122,7 @@
     </row>
     <row r="105" spans="1:13">
       <c r="A105" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -2899,7 +3139,7 @@
     </row>
     <row r="106" spans="1:13">
       <c r="A106" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2916,7 +3156,7 @@
     </row>
     <row r="107" spans="1:13">
       <c r="A107" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -2933,7 +3173,7 @@
     </row>
     <row r="108" spans="1:13">
       <c r="A108" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -2950,7 +3190,7 @@
     </row>
     <row r="109" spans="1:13">
       <c r="A109" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -2967,7 +3207,7 @@
     </row>
     <row r="110" spans="1:13">
       <c r="A110" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -2984,7 +3224,7 @@
     </row>
     <row r="111" spans="1:13">
       <c r="A111" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -3001,7 +3241,7 @@
     </row>
     <row r="112" spans="1:13">
       <c r="A112" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3018,7 +3258,7 @@
     </row>
     <row r="113" spans="1:13">
       <c r="A113" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3035,7 +3275,7 @@
     </row>
     <row r="114" spans="1:13">
       <c r="A114" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -3052,7 +3292,7 @@
     </row>
     <row r="115" spans="1:13">
       <c r="A115" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3069,7 +3309,7 @@
     </row>
     <row r="116" spans="1:13">
       <c r="A116" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3086,7 +3326,7 @@
     </row>
     <row r="117" spans="1:13">
       <c r="A117" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3103,7 +3343,7 @@
     </row>
     <row r="118" spans="1:13">
       <c r="A118" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3120,7 +3360,7 @@
     </row>
     <row r="119" spans="1:13">
       <c r="A119" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3137,7 +3377,7 @@
     </row>
     <row r="120" spans="1:13">
       <c r="A120" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3154,7 +3394,7 @@
     </row>
     <row r="121" spans="1:13">
       <c r="A121" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3171,7 +3411,7 @@
     </row>
     <row r="122" spans="1:13">
       <c r="A122" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3188,7 +3428,7 @@
     </row>
     <row r="123" spans="1:13">
       <c r="A123" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3205,7 +3445,7 @@
     </row>
     <row r="124" spans="1:13">
       <c r="A124" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3222,7 +3462,7 @@
     </row>
     <row r="125" spans="1:13">
       <c r="A125" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3239,7 +3479,7 @@
     </row>
     <row r="126" spans="1:13">
       <c r="A126" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -3256,7 +3496,7 @@
     </row>
     <row r="127" spans="1:13">
       <c r="A127" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3273,7 +3513,7 @@
     </row>
     <row r="128" spans="1:13">
       <c r="A128" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3290,7 +3530,7 @@
     </row>
     <row r="129" spans="1:13">
       <c r="A129" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3307,7 +3547,7 @@
     </row>
     <row r="130" spans="1:13">
       <c r="A130" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -3324,7 +3564,7 @@
     </row>
     <row r="131" spans="1:13">
       <c r="A131" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3341,7 +3581,7 @@
     </row>
     <row r="132" spans="1:13">
       <c r="A132" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3358,7 +3598,7 @@
     </row>
     <row r="133" spans="1:13">
       <c r="A133" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3375,7 +3615,7 @@
     </row>
     <row r="134" spans="1:13">
       <c r="A134" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3392,7 +3632,7 @@
     </row>
     <row r="135" spans="1:13">
       <c r="A135" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3409,7 +3649,7 @@
     </row>
     <row r="136" spans="1:13">
       <c r="A136" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3426,7 +3666,7 @@
     </row>
     <row r="137" spans="1:13">
       <c r="A137" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3443,7 +3683,7 @@
     </row>
     <row r="138" spans="1:13">
       <c r="A138" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3460,7 +3700,7 @@
     </row>
     <row r="139" spans="1:13">
       <c r="A139" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3477,7 +3717,7 @@
     </row>
     <row r="140" spans="1:13">
       <c r="A140" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3494,7 +3734,7 @@
     </row>
     <row r="141" spans="1:13">
       <c r="A141" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3511,7 +3751,7 @@
     </row>
     <row r="142" spans="1:13">
       <c r="A142" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3528,7 +3768,7 @@
     </row>
     <row r="143" spans="1:13">
       <c r="A143" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3545,7 +3785,7 @@
     </row>
     <row r="144" spans="1:13">
       <c r="A144" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3562,7 +3802,7 @@
     </row>
     <row r="145" spans="1:13">
       <c r="A145" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3579,7 +3819,7 @@
     </row>
     <row r="146" spans="1:13">
       <c r="A146" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3596,7 +3836,7 @@
     </row>
     <row r="147" spans="1:13">
       <c r="A147" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -3613,7 +3853,7 @@
     </row>
     <row r="148" spans="1:13">
       <c r="A148" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -3630,7 +3870,7 @@
     </row>
     <row r="149" spans="1:13">
       <c r="A149" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -3647,7 +3887,7 @@
     </row>
     <row r="150" spans="1:13">
       <c r="A150" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -3664,7 +3904,7 @@
     </row>
     <row r="151" spans="1:13">
       <c r="A151" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -3681,7 +3921,7 @@
     </row>
     <row r="152" spans="1:13">
       <c r="A152" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -3698,7 +3938,7 @@
     </row>
     <row r="153" spans="1:13">
       <c r="A153" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -3715,7 +3955,7 @@
     </row>
     <row r="154" spans="1:13">
       <c r="A154" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -3732,7 +3972,7 @@
     </row>
     <row r="155" spans="1:13">
       <c r="A155" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -3749,7 +3989,7 @@
     </row>
     <row r="156" spans="1:13">
       <c r="A156" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -3766,7 +4006,7 @@
     </row>
     <row r="157" spans="1:13">
       <c r="A157" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -3783,7 +4023,7 @@
     </row>
     <row r="158" spans="1:13">
       <c r="A158" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -3800,7 +4040,7 @@
     </row>
     <row r="159" spans="1:13">
       <c r="A159" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -3817,7 +4057,7 @@
     </row>
     <row r="160" spans="1:13">
       <c r="A160" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -3834,7 +4074,7 @@
     </row>
     <row r="161" spans="1:13">
       <c r="A161" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -3851,7 +4091,7 @@
     </row>
     <row r="162" spans="1:13">
       <c r="A162" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -3868,7 +4108,7 @@
     </row>
     <row r="163" spans="1:13">
       <c r="A163" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -3885,7 +4125,7 @@
     </row>
     <row r="164" spans="1:13">
       <c r="A164" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -3902,7 +4142,7 @@
     </row>
     <row r="165" spans="1:13">
       <c r="A165" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -3919,7 +4159,7 @@
     </row>
     <row r="166" spans="1:13">
       <c r="A166" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -3936,7 +4176,7 @@
     </row>
     <row r="167" spans="1:13">
       <c r="A167" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -3953,7 +4193,7 @@
     </row>
     <row r="168" spans="1:13">
       <c r="A168" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -3970,7 +4210,7 @@
     </row>
     <row r="169" spans="1:13">
       <c r="A169" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -3987,7 +4227,7 @@
     </row>
     <row r="170" spans="1:13">
       <c r="A170" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -4004,7 +4244,7 @@
     </row>
     <row r="171" spans="1:13">
       <c r="A171" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -4021,7 +4261,7 @@
     </row>
     <row r="172" spans="1:13">
       <c r="A172" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -4038,7 +4278,7 @@
     </row>
     <row r="173" spans="1:13">
       <c r="A173" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -4055,7 +4295,7 @@
     </row>
     <row r="174" spans="1:13">
       <c r="A174" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -4072,7 +4312,7 @@
     </row>
     <row r="175" spans="1:13">
       <c r="A175" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -4089,7 +4329,7 @@
     </row>
     <row r="176" spans="1:13">
       <c r="A176" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -4106,7 +4346,7 @@
     </row>
     <row r="177" spans="1:13">
       <c r="A177" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -4123,7 +4363,7 @@
     </row>
     <row r="178" spans="1:13">
       <c r="A178" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -4140,7 +4380,7 @@
     </row>
     <row r="179" spans="1:13">
       <c r="A179" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -4157,7 +4397,7 @@
     </row>
     <row r="180" spans="1:13">
       <c r="A180" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -4174,7 +4414,7 @@
     </row>
     <row r="181" spans="1:13">
       <c r="A181" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -4191,7 +4431,7 @@
     </row>
     <row r="182" spans="1:13">
       <c r="A182" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -4208,7 +4448,7 @@
     </row>
     <row r="183" spans="1:13">
       <c r="A183" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -4225,7 +4465,7 @@
     </row>
     <row r="184" spans="1:13">
       <c r="A184" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -4242,7 +4482,7 @@
     </row>
     <row r="185" spans="1:13">
       <c r="A185" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -4259,7 +4499,7 @@
     </row>
     <row r="186" spans="1:13">
       <c r="A186" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -4276,7 +4516,7 @@
     </row>
     <row r="187" spans="1:13">
       <c r="A187" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -4293,7 +4533,7 @@
     </row>
     <row r="188" spans="1:13">
       <c r="A188" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -4310,7 +4550,7 @@
     </row>
     <row r="189" spans="1:13">
       <c r="A189" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -4327,7 +4567,7 @@
     </row>
     <row r="190" spans="1:13">
       <c r="A190" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -4344,7 +4584,7 @@
     </row>
     <row r="191" spans="1:13">
       <c r="A191" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -4361,7 +4601,7 @@
     </row>
     <row r="192" spans="1:13">
       <c r="A192" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -4378,7 +4618,7 @@
     </row>
     <row r="193" spans="1:13">
       <c r="A193" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -4395,7 +4635,7 @@
     </row>
     <row r="194" spans="1:13">
       <c r="A194" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -4412,7 +4652,7 @@
     </row>
     <row r="195" spans="1:13">
       <c r="A195" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -4429,7 +4669,7 @@
     </row>
     <row r="196" spans="1:13">
       <c r="A196" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -4446,7 +4686,7 @@
     </row>
     <row r="197" spans="1:13">
       <c r="A197" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -4463,7 +4703,7 @@
     </row>
     <row r="198" spans="1:13">
       <c r="A198" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -4480,7 +4720,7 @@
     </row>
     <row r="199" spans="1:13">
       <c r="A199" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -4497,7 +4737,7 @@
     </row>
     <row r="200" spans="1:13">
       <c r="A200" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -4514,7 +4754,7 @@
     </row>
     <row r="201" spans="1:13">
       <c r="A201" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -4531,7 +4771,7 @@
     </row>
     <row r="202" spans="1:13">
       <c r="A202" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
@@ -4548,7 +4788,7 @@
     </row>
     <row r="203" spans="1:13">
       <c r="A203" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -4565,7 +4805,7 @@
     </row>
     <row r="204" spans="1:13">
       <c r="A204" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
@@ -4582,7 +4822,7 @@
     </row>
     <row r="205" spans="1:13">
       <c r="A205" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
@@ -4599,7 +4839,7 @@
     </row>
     <row r="206" spans="1:13">
       <c r="A206" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
@@ -4616,7 +4856,7 @@
     </row>
     <row r="207" spans="1:13">
       <c r="A207" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
@@ -4633,7 +4873,7 @@
     </row>
     <row r="208" spans="1:13">
       <c r="A208" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
@@ -4650,7 +4890,7 @@
     </row>
     <row r="209" spans="1:13">
       <c r="A209" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
@@ -4667,7 +4907,7 @@
     </row>
     <row r="210" spans="1:13">
       <c r="A210" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
@@ -4684,7 +4924,7 @@
     </row>
     <row r="211" spans="1:13">
       <c r="A211" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
@@ -4701,7 +4941,7 @@
     </row>
     <row r="212" spans="1:13">
       <c r="A212" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
@@ -4718,7 +4958,7 @@
     </row>
     <row r="213" spans="1:13">
       <c r="A213" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
@@ -4735,7 +4975,7 @@
     </row>
     <row r="214" spans="1:13">
       <c r="A214" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
@@ -4752,7 +4992,7 @@
     </row>
     <row r="215" spans="1:13">
       <c r="A215" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
@@ -4769,7 +5009,7 @@
     </row>
     <row r="216" spans="1:13">
       <c r="A216" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
@@ -4786,7 +5026,7 @@
     </row>
     <row r="217" spans="1:13">
       <c r="A217" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
@@ -4803,7 +5043,7 @@
     </row>
     <row r="218" spans="1:13">
       <c r="A218" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
@@ -4820,7 +5060,7 @@
     </row>
     <row r="219" spans="1:13">
       <c r="A219" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
@@ -4837,7 +5077,7 @@
     </row>
     <row r="220" spans="1:13">
       <c r="A220" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
@@ -4854,7 +5094,7 @@
     </row>
     <row r="221" spans="1:13">
       <c r="A221" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
@@ -4871,7 +5111,7 @@
     </row>
     <row r="222" spans="1:13">
       <c r="A222" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
@@ -4888,7 +5128,7 @@
     </row>
     <row r="223" spans="1:13">
       <c r="A223" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
@@ -4905,7 +5145,7 @@
     </row>
     <row r="224" spans="1:13">
       <c r="A224" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
@@ -4922,7 +5162,7 @@
     </row>
     <row r="225" spans="1:13">
       <c r="A225" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>

</xml_diff>

<commit_message>
? replaced by 0 in Excel
</commit_message>
<xml_diff>
--- a/labellisation.xlsx
+++ b/labellisation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nizon\Documents\Perso\Cours\Cours 4A\The AI Lifecycle\App-For-People-With-Restricted-Diet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE042F9-E229-4EC7-8EC9-8D099243817F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6619F5-680F-4078-A779-8076EF086BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="239">
   <si>
     <t>Name</t>
   </si>
@@ -752,7 +752,7 @@
     <t>molluscs</t>
   </si>
   <si>
-    <t>consider "traces of"</t>
+    <t>consider "traces of".</t>
   </si>
 </sst>
 </file>
@@ -816,7 +816,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -825,10 +825,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1110,7 +1109,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N1" sqref="N1"/>
+      <selection pane="bottomLeft" sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -1165,16 +1164,16 @@
       <c r="K3" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="1" t="s">
         <v>232</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="1" t="s">
         <v>235</v>
       </c>
     </row>
@@ -2357,47 +2356,47 @@
       <c r="A29" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>236</v>
+      <c r="B29" s="1">
+        <v>0</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0</v>
       </c>
       <c r="G29" s="1">
         <v>1</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>236</v>
+      <c r="H29" s="1">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0</v>
+      </c>
+      <c r="L29" s="1">
+        <v>0</v>
+      </c>
+      <c r="M29" s="1">
+        <v>0</v>
+      </c>
+      <c r="N29" s="1">
+        <v>0</v>
+      </c>
+      <c r="O29" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -2407,44 +2406,44 @@
       <c r="B30" s="1">
         <v>1</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>236</v>
+      <c r="C30" s="1">
+        <v>0</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>236</v>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
       </c>
       <c r="G30" s="1">
         <v>1</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="N30" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="O30" s="1" t="s">
-        <v>236</v>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0</v>
+      </c>
+      <c r="L30" s="1">
+        <v>0</v>
+      </c>
+      <c r="M30" s="1">
+        <v>0</v>
+      </c>
+      <c r="N30" s="1">
+        <v>0</v>
+      </c>
+      <c r="O30" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:15">
@@ -11587,60 +11586,60 @@
       </c>
     </row>
     <row r="226" spans="1:15">
-      <c r="B226">
-        <f>SUM(B4:B225)</f>
+      <c r="B226" s="1">
+        <f t="shared" ref="B226:O226" si="0">SUM(B4:B225)</f>
         <v>112</v>
       </c>
-      <c r="C226">
-        <f>SUM(C4:C225)</f>
+      <c r="C226" s="1">
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="D226">
-        <f>SUM(D4:D225)</f>
+      <c r="D226" s="1">
+        <f t="shared" si="0"/>
         <v>107</v>
       </c>
-      <c r="E226">
-        <f>SUM(E4:E225)</f>
+      <c r="E226" s="1">
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="F226">
-        <f>SUM(F4:F225)</f>
+      <c r="F226" s="1">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="G226">
-        <f>SUM(G4:G225)</f>
+      <c r="G226" s="1">
+        <f t="shared" si="0"/>
         <v>105</v>
       </c>
-      <c r="H226">
-        <f>SUM(H4:H225)</f>
-        <v>0</v>
-      </c>
-      <c r="I226">
-        <f>SUM(I4:I225)</f>
+      <c r="H226" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I226" s="1">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="J226">
-        <f>SUM(J4:J225)</f>
-        <v>0</v>
-      </c>
-      <c r="K226">
-        <f>SUM(K4:K225)</f>
+      <c r="J226" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K226" s="1">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="L226">
-        <f>SUM(L4:L225)</f>
+      <c r="L226" s="1">
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="M226">
-        <f>SUM(M4:M225)</f>
+      <c r="M226" s="1">
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="N226">
-        <f>SUM(N4:N225)</f>
+      <c r="N226" s="1">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="O226">
-        <f>SUM(O4:O225)</f>
+      <c r="O226" s="1">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Excel modified. More details/stats
</commit_message>
<xml_diff>
--- a/labellisation.xlsx
+++ b/labellisation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nizon\Documents\Perso\Cours\Cours 4A\The AI Lifecycle\App-For-People-With-Restricted-Diet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27BDFFDE-3AE4-4F20-9590-96AB218D1EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CAC6CD-FCB2-4A06-8920-0B59FCF6E355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="238">
   <si>
     <t>Name</t>
   </si>
@@ -741,6 +741,15 @@
   </si>
   <si>
     <t>consider "traces of"</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Average number of allergen per product</t>
+  </si>
+  <si>
+    <t>Number of products containing n allergens</t>
   </si>
 </sst>
 </file>
@@ -777,7 +786,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -800,11 +809,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -813,9 +863,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1093,16 +1148,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O223"/>
+  <dimension ref="A1:P243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A217" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O223" sqref="O223"/>
+      <pane ySplit="3" topLeftCell="A222" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N234" sqref="N234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" s="3" t="s">
         <v>234</v>
       </c>
@@ -1118,7 +1173,7 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1164,8 +1219,11 @@
       <c r="O3" s="1" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="P3" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1185,7 +1243,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
@@ -1211,8 +1269,12 @@
       <c r="O4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="P4" s="1">
+        <f>SUM(B4:O4)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1258,8 +1320,12 @@
       <c r="O5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="P5" s="1">
+        <f>SUM(B5:O5)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1305,8 +1371,12 @@
       <c r="O6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="P6" s="1">
+        <f t="shared" ref="P6:P69" si="0">SUM(B6:O6)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1352,8 +1422,12 @@
       <c r="O7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="P7" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1399,8 +1473,12 @@
       <c r="O8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="P8" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1446,8 +1524,12 @@
       <c r="O9" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="P9" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1493,8 +1575,12 @@
       <c r="O10" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="P10" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -1540,8 +1626,12 @@
       <c r="O11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="P11" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1587,8 +1677,12 @@
       <c r="O12" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="P12" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -1634,8 +1728,12 @@
       <c r="O13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="P13" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
@@ -1681,8 +1779,12 @@
       <c r="O14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="P14" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -1728,8 +1830,12 @@
       <c r="O15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="P15" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
@@ -1775,8 +1881,12 @@
       <c r="O16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="P16" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
@@ -1822,8 +1932,12 @@
       <c r="O17" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="P17" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -1869,8 +1983,12 @@
       <c r="O18" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="P18" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -1916,8 +2034,12 @@
       <c r="O19" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="P19" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -1963,8 +2085,12 @@
       <c r="O20" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="P20" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -2010,8 +2136,12 @@
       <c r="O21" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="P21" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -2057,8 +2187,12 @@
       <c r="O22" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="P22" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
@@ -2104,8 +2238,12 @@
       <c r="O23" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="P23" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
@@ -2151,8 +2289,12 @@
       <c r="O24" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="P24" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
@@ -2198,8 +2340,12 @@
       <c r="O25" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="P25" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" s="2" t="s">
         <v>28</v>
       </c>
@@ -2245,8 +2391,12 @@
       <c r="O26" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="P26" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" s="2" t="s">
         <v>29</v>
       </c>
@@ -2292,8 +2442,12 @@
       <c r="O27" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="P27" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
@@ -2339,8 +2493,12 @@
       <c r="O28" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="P28" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" s="2" t="s">
         <v>31</v>
       </c>
@@ -2386,8 +2544,12 @@
       <c r="O29" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="P29" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" s="2" t="s">
         <v>32</v>
       </c>
@@ -2433,8 +2595,12 @@
       <c r="O30" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="P30" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" s="2" t="s">
         <v>33</v>
       </c>
@@ -2480,8 +2646,12 @@
       <c r="O31" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:15">
+      <c r="P31" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" s="2" t="s">
         <v>34</v>
       </c>
@@ -2527,8 +2697,12 @@
       <c r="O32" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="P32" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" s="2" t="s">
         <v>35</v>
       </c>
@@ -2574,8 +2748,12 @@
       <c r="O33" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="P33" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" s="2" t="s">
         <v>36</v>
       </c>
@@ -2621,8 +2799,12 @@
       <c r="O34" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:15">
+      <c r="P34" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35" s="2" t="s">
         <v>37</v>
       </c>
@@ -2668,8 +2850,12 @@
       <c r="O35" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="P35" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36" s="2" t="s">
         <v>38</v>
       </c>
@@ -2715,8 +2901,12 @@
       <c r="O36" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="P36" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
@@ -2762,8 +2952,12 @@
       <c r="O37" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:15">
+      <c r="P37" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
       <c r="A38" s="2" t="s">
         <v>40</v>
       </c>
@@ -2809,8 +3003,12 @@
       <c r="O38" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:15">
+      <c r="P38" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
       <c r="A39" s="2" t="s">
         <v>41</v>
       </c>
@@ -2856,8 +3054,12 @@
       <c r="O39" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:15">
+      <c r="P39" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40" s="2" t="s">
         <v>42</v>
       </c>
@@ -2903,8 +3105,12 @@
       <c r="O40" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:15">
+      <c r="P40" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
       <c r="A41" s="2" t="s">
         <v>43</v>
       </c>
@@ -2950,8 +3156,12 @@
       <c r="O41" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:15">
+      <c r="P41" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
       <c r="A42" s="2" t="s">
         <v>44</v>
       </c>
@@ -2997,8 +3207,12 @@
       <c r="O42" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:15">
+      <c r="P42" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
       <c r="A43" s="2" t="s">
         <v>45</v>
       </c>
@@ -3044,8 +3258,12 @@
       <c r="O43" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:15">
+      <c r="P43" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
       <c r="A44" s="2" t="s">
         <v>46</v>
       </c>
@@ -3091,8 +3309,12 @@
       <c r="O44" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:15">
+      <c r="P44" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
       <c r="A45" s="2" t="s">
         <v>47</v>
       </c>
@@ -3138,8 +3360,12 @@
       <c r="O45" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:15">
+      <c r="P45" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
       <c r="A46" s="2" t="s">
         <v>48</v>
       </c>
@@ -3185,8 +3411,12 @@
       <c r="O46" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:15">
+      <c r="P46" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
       <c r="A47" s="2" t="s">
         <v>49</v>
       </c>
@@ -3232,8 +3462,12 @@
       <c r="O47" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:15">
+      <c r="P47" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
       <c r="A48" s="2" t="s">
         <v>50</v>
       </c>
@@ -3279,8 +3513,12 @@
       <c r="O48" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:15">
+      <c r="P48" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
       <c r="A49" s="2" t="s">
         <v>51</v>
       </c>
@@ -3326,8 +3564,12 @@
       <c r="O49" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:15">
+      <c r="P49" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16">
       <c r="A50" s="2" t="s">
         <v>52</v>
       </c>
@@ -3373,8 +3615,12 @@
       <c r="O50" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:15">
+      <c r="P50" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
       <c r="A51" s="2" t="s">
         <v>53</v>
       </c>
@@ -3420,8 +3666,12 @@
       <c r="O51" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:15">
+      <c r="P51" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
       <c r="A52" s="2" t="s">
         <v>54</v>
       </c>
@@ -3467,8 +3717,12 @@
       <c r="O52" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:15">
+      <c r="P52" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
       <c r="A53" s="2" t="s">
         <v>55</v>
       </c>
@@ -3514,8 +3768,12 @@
       <c r="O53" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:15">
+      <c r="P53" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
       <c r="A54" s="2" t="s">
         <v>56</v>
       </c>
@@ -3561,8 +3819,12 @@
       <c r="O54" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:15">
+      <c r="P54" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
       <c r="A55" s="2" t="s">
         <v>57</v>
       </c>
@@ -3608,8 +3870,12 @@
       <c r="O55" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:15">
+      <c r="P55" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16">
       <c r="A56" s="2" t="s">
         <v>58</v>
       </c>
@@ -3655,8 +3921,12 @@
       <c r="O56" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:15">
+      <c r="P56" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
       <c r="A57" s="2" t="s">
         <v>59</v>
       </c>
@@ -3702,8 +3972,12 @@
       <c r="O57" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:15">
+      <c r="P57" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16">
       <c r="A58" s="2" t="s">
         <v>60</v>
       </c>
@@ -3749,8 +4023,12 @@
       <c r="O58" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:15">
+      <c r="P58" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16">
       <c r="A59" s="2" t="s">
         <v>61</v>
       </c>
@@ -3796,8 +4074,12 @@
       <c r="O59" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:15">
+      <c r="P59" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16">
       <c r="A60" s="2" t="s">
         <v>62</v>
       </c>
@@ -3843,8 +4125,12 @@
       <c r="O60" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:15">
+      <c r="P60" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16">
       <c r="A61" s="2" t="s">
         <v>63</v>
       </c>
@@ -3890,8 +4176,12 @@
       <c r="O61" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:15">
+      <c r="P61" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16">
       <c r="A62" s="2" t="s">
         <v>64</v>
       </c>
@@ -3937,8 +4227,12 @@
       <c r="O62" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:15">
+      <c r="P62" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
       <c r="A63" s="2" t="s">
         <v>65</v>
       </c>
@@ -3984,8 +4278,12 @@
       <c r="O63" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:15">
+      <c r="P63" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16">
       <c r="A64" s="2" t="s">
         <v>66</v>
       </c>
@@ -4031,8 +4329,12 @@
       <c r="O64" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:15">
+      <c r="P64" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16">
       <c r="A65" s="2" t="s">
         <v>67</v>
       </c>
@@ -4078,8 +4380,12 @@
       <c r="O65" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:15">
+      <c r="P65" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16">
       <c r="A66" s="2" t="s">
         <v>68</v>
       </c>
@@ -4125,8 +4431,12 @@
       <c r="O66" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:15">
+      <c r="P66" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16">
       <c r="A67" s="2" t="s">
         <v>69</v>
       </c>
@@ -4172,8 +4482,12 @@
       <c r="O67" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:15">
+      <c r="P67" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16">
       <c r="A68" s="2" t="s">
         <v>70</v>
       </c>
@@ -4219,8 +4533,12 @@
       <c r="O68" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:15">
+      <c r="P68" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16">
       <c r="A69" s="2" t="s">
         <v>71</v>
       </c>
@@ -4266,8 +4584,12 @@
       <c r="O69" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:15">
+      <c r="P69" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16">
       <c r="A70" s="2" t="s">
         <v>72</v>
       </c>
@@ -4313,8 +4635,12 @@
       <c r="O70" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:15">
+      <c r="P70" s="1">
+        <f t="shared" ref="P70:P133" si="1">SUM(B70:O70)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16">
       <c r="A71" s="2" t="s">
         <v>73</v>
       </c>
@@ -4360,8 +4686,12 @@
       <c r="O71" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:15">
+      <c r="P71" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16">
       <c r="A72" s="2" t="s">
         <v>74</v>
       </c>
@@ -4407,8 +4737,12 @@
       <c r="O72" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:15">
+      <c r="P72" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16">
       <c r="A73" s="2" t="s">
         <v>75</v>
       </c>
@@ -4454,8 +4788,12 @@
       <c r="O73" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:15">
+      <c r="P73" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16">
       <c r="A74" s="2" t="s">
         <v>76</v>
       </c>
@@ -4501,8 +4839,12 @@
       <c r="O74" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:15">
+      <c r="P74" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16">
       <c r="A75" s="2" t="s">
         <v>77</v>
       </c>
@@ -4548,8 +4890,12 @@
       <c r="O75" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:15">
+      <c r="P75" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16">
       <c r="A76" s="2" t="s">
         <v>78</v>
       </c>
@@ -4595,8 +4941,12 @@
       <c r="O76" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:15">
+      <c r="P76" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16">
       <c r="A77" s="2" t="s">
         <v>79</v>
       </c>
@@ -4642,8 +4992,12 @@
       <c r="O77" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:15">
+      <c r="P77" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16">
       <c r="A78" s="2" t="s">
         <v>80</v>
       </c>
@@ -4689,8 +5043,12 @@
       <c r="O78" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:15">
+      <c r="P78" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16">
       <c r="A79" s="2" t="s">
         <v>81</v>
       </c>
@@ -4736,8 +5094,12 @@
       <c r="O79" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:15">
+      <c r="P79" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16">
       <c r="A80" s="2" t="s">
         <v>82</v>
       </c>
@@ -4783,8 +5145,12 @@
       <c r="O80" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:15">
+      <c r="P80" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16">
       <c r="A81" s="2" t="s">
         <v>83</v>
       </c>
@@ -4830,8 +5196,12 @@
       <c r="O81" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:15">
+      <c r="P81" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16">
       <c r="A82" s="2" t="s">
         <v>84</v>
       </c>
@@ -4877,8 +5247,12 @@
       <c r="O82" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:15">
+      <c r="P82" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16">
       <c r="A83" s="2" t="s">
         <v>85</v>
       </c>
@@ -4924,8 +5298,12 @@
       <c r="O83" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:15">
+      <c r="P83" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16">
       <c r="A84" s="2" t="s">
         <v>86</v>
       </c>
@@ -4971,8 +5349,12 @@
       <c r="O84" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:15">
+      <c r="P84" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16">
       <c r="A85" s="2" t="s">
         <v>87</v>
       </c>
@@ -5018,8 +5400,12 @@
       <c r="O85" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:15">
+      <c r="P85" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16">
       <c r="A86" s="2" t="s">
         <v>88</v>
       </c>
@@ -5065,8 +5451,12 @@
       <c r="O86" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:15">
+      <c r="P86" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16">
       <c r="A87" s="2" t="s">
         <v>89</v>
       </c>
@@ -5112,8 +5502,12 @@
       <c r="O87" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:15">
+      <c r="P87" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16">
       <c r="A88" s="2" t="s">
         <v>90</v>
       </c>
@@ -5159,8 +5553,12 @@
       <c r="O88" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:15">
+      <c r="P88" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16">
       <c r="A89" s="2" t="s">
         <v>91</v>
       </c>
@@ -5206,8 +5604,12 @@
       <c r="O89" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:15">
+      <c r="P89" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16">
       <c r="A90" s="2" t="s">
         <v>92</v>
       </c>
@@ -5253,8 +5655,12 @@
       <c r="O90" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:15">
+      <c r="P90" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16">
       <c r="A91" s="2" t="s">
         <v>93</v>
       </c>
@@ -5300,8 +5706,12 @@
       <c r="O91" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:15">
+      <c r="P91" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16">
       <c r="A92" s="2" t="s">
         <v>94</v>
       </c>
@@ -5347,8 +5757,12 @@
       <c r="O92" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:15">
+      <c r="P92" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16">
       <c r="A93" s="2" t="s">
         <v>95</v>
       </c>
@@ -5394,8 +5808,12 @@
       <c r="O93" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:15">
+      <c r="P93" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16">
       <c r="A94" s="2" t="s">
         <v>96</v>
       </c>
@@ -5441,8 +5859,12 @@
       <c r="O94" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:15">
+      <c r="P94" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16">
       <c r="A95" s="2" t="s">
         <v>97</v>
       </c>
@@ -5488,8 +5910,12 @@
       <c r="O95" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:15">
+      <c r="P95" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16">
       <c r="A96" s="2" t="s">
         <v>98</v>
       </c>
@@ -5535,8 +5961,12 @@
       <c r="O96" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:15">
+      <c r="P96" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16">
       <c r="A97" s="2" t="s">
         <v>99</v>
       </c>
@@ -5582,8 +6012,12 @@
       <c r="O97" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:15">
+      <c r="P97" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16">
       <c r="A98" s="2" t="s">
         <v>100</v>
       </c>
@@ -5629,8 +6063,12 @@
       <c r="O98" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:15">
+      <c r="P98" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16">
       <c r="A99" s="2" t="s">
         <v>101</v>
       </c>
@@ -5676,8 +6114,12 @@
       <c r="O99" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:15">
+      <c r="P99" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16">
       <c r="A100" s="2" t="s">
         <v>102</v>
       </c>
@@ -5723,8 +6165,12 @@
       <c r="O100" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:15">
+      <c r="P100" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16">
       <c r="A101" s="2" t="s">
         <v>103</v>
       </c>
@@ -5770,8 +6216,12 @@
       <c r="O101" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:15">
+      <c r="P101" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16">
       <c r="A102" s="2" t="s">
         <v>104</v>
       </c>
@@ -5817,8 +6267,12 @@
       <c r="O102" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:15">
+      <c r="P102" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16">
       <c r="A103" s="2" t="s">
         <v>105</v>
       </c>
@@ -5864,8 +6318,12 @@
       <c r="O103" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:15">
+      <c r="P103" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16">
       <c r="A104" s="2" t="s">
         <v>106</v>
       </c>
@@ -5911,8 +6369,12 @@
       <c r="O104" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:15">
+      <c r="P104" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16">
       <c r="A105" s="2" t="s">
         <v>107</v>
       </c>
@@ -5958,8 +6420,12 @@
       <c r="O105" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:15">
+      <c r="P105" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16">
       <c r="A106" s="2" t="s">
         <v>108</v>
       </c>
@@ -6005,8 +6471,12 @@
       <c r="O106" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:15">
+      <c r="P106" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16">
       <c r="A107" s="2" t="s">
         <v>109</v>
       </c>
@@ -6052,8 +6522,12 @@
       <c r="O107" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:15">
+      <c r="P107" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16">
       <c r="A108" s="2" t="s">
         <v>110</v>
       </c>
@@ -6099,8 +6573,12 @@
       <c r="O108" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:15">
+      <c r="P108" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16">
       <c r="A109" s="2" t="s">
         <v>111</v>
       </c>
@@ -6146,8 +6624,12 @@
       <c r="O109" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:15">
+      <c r="P109" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16">
       <c r="A110" s="2" t="s">
         <v>112</v>
       </c>
@@ -6193,8 +6675,12 @@
       <c r="O110" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:15">
+      <c r="P110" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16">
       <c r="A111" s="2" t="s">
         <v>113</v>
       </c>
@@ -6240,8 +6726,12 @@
       <c r="O111" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:15">
+      <c r="P111" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16">
       <c r="A112" s="2" t="s">
         <v>114</v>
       </c>
@@ -6287,8 +6777,12 @@
       <c r="O112" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:15">
+      <c r="P112" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16">
       <c r="A113" s="2" t="s">
         <v>115</v>
       </c>
@@ -6334,8 +6828,12 @@
       <c r="O113" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:15">
+      <c r="P113" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16">
       <c r="A114" s="2" t="s">
         <v>116</v>
       </c>
@@ -6381,8 +6879,12 @@
       <c r="O114" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:15">
+      <c r="P114" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16">
       <c r="A115" s="2" t="s">
         <v>117</v>
       </c>
@@ -6428,8 +6930,12 @@
       <c r="O115" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:15">
+      <c r="P115" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16">
       <c r="A116" s="2" t="s">
         <v>118</v>
       </c>
@@ -6475,8 +6981,12 @@
       <c r="O116" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:15">
+      <c r="P116" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16">
       <c r="A117" s="2" t="s">
         <v>119</v>
       </c>
@@ -6522,8 +7032,12 @@
       <c r="O117" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:15">
+      <c r="P117" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16">
       <c r="A118" s="2" t="s">
         <v>120</v>
       </c>
@@ -6569,8 +7083,12 @@
       <c r="O118" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:15">
+      <c r="P118" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16">
       <c r="A119" s="2" t="s">
         <v>121</v>
       </c>
@@ -6616,8 +7134,12 @@
       <c r="O119" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:15">
+      <c r="P119" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16">
       <c r="A120" s="2" t="s">
         <v>122</v>
       </c>
@@ -6663,8 +7185,12 @@
       <c r="O120" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:15">
+      <c r="P120" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16">
       <c r="A121" s="2" t="s">
         <v>123</v>
       </c>
@@ -6710,8 +7236,12 @@
       <c r="O121" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:15">
+      <c r="P121" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16">
       <c r="A122" s="2" t="s">
         <v>124</v>
       </c>
@@ -6757,8 +7287,12 @@
       <c r="O122" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:15">
+      <c r="P122" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16">
       <c r="A123" s="2" t="s">
         <v>125</v>
       </c>
@@ -6804,8 +7338,12 @@
       <c r="O123" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:15">
+      <c r="P123" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16">
       <c r="A124" s="2" t="s">
         <v>126</v>
       </c>
@@ -6851,8 +7389,12 @@
       <c r="O124" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:15">
+      <c r="P124" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16">
       <c r="A125" s="2" t="s">
         <v>127</v>
       </c>
@@ -6898,8 +7440,12 @@
       <c r="O125" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:15">
+      <c r="P125" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16">
       <c r="A126" s="2" t="s">
         <v>128</v>
       </c>
@@ -6945,8 +7491,12 @@
       <c r="O126" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:15">
+      <c r="P126" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16">
       <c r="A127" s="2" t="s">
         <v>129</v>
       </c>
@@ -6992,8 +7542,12 @@
       <c r="O127" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:15">
+      <c r="P127" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16">
       <c r="A128" s="2" t="s">
         <v>130</v>
       </c>
@@ -7039,8 +7593,12 @@
       <c r="O128" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:15">
+      <c r="P128" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:16">
       <c r="A129" s="2" t="s">
         <v>131</v>
       </c>
@@ -7086,8 +7644,12 @@
       <c r="O129" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:15">
+      <c r="P129" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:16">
       <c r="A130" s="2" t="s">
         <v>132</v>
       </c>
@@ -7133,8 +7695,12 @@
       <c r="O130" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:15">
+      <c r="P130" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:16">
       <c r="A131" s="2" t="s">
         <v>133</v>
       </c>
@@ -7180,8 +7746,12 @@
       <c r="O131" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:15">
+      <c r="P131" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:16">
       <c r="A132" s="2" t="s">
         <v>134</v>
       </c>
@@ -7227,8 +7797,12 @@
       <c r="O132" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:15">
+      <c r="P132" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:16">
       <c r="A133" s="2" t="s">
         <v>135</v>
       </c>
@@ -7274,8 +7848,12 @@
       <c r="O133" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:15">
+      <c r="P133" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16">
       <c r="A134" s="2" t="s">
         <v>136</v>
       </c>
@@ -7321,8 +7899,12 @@
       <c r="O134" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:15">
+      <c r="P134" s="1">
+        <f t="shared" ref="P134:P197" si="2">SUM(B134:O134)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16">
       <c r="A135" s="2" t="s">
         <v>137</v>
       </c>
@@ -7368,8 +7950,12 @@
       <c r="O135" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:15">
+      <c r="P135" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16">
       <c r="A136" s="2" t="s">
         <v>138</v>
       </c>
@@ -7415,8 +8001,12 @@
       <c r="O136" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:15">
+      <c r="P136" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16">
       <c r="A137" s="2" t="s">
         <v>139</v>
       </c>
@@ -7462,8 +8052,12 @@
       <c r="O137" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:15">
+      <c r="P137" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:16">
       <c r="A138" s="2" t="s">
         <v>140</v>
       </c>
@@ -7509,8 +8103,12 @@
       <c r="O138" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:15">
+      <c r="P138" s="1">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16">
       <c r="A139" s="2" t="s">
         <v>141</v>
       </c>
@@ -7556,8 +8154,12 @@
       <c r="O139" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:15">
+      <c r="P139" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16">
       <c r="A140" s="2" t="s">
         <v>142</v>
       </c>
@@ -7603,8 +8205,12 @@
       <c r="O140" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:15">
+      <c r="P140" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16">
       <c r="A141" s="2" t="s">
         <v>143</v>
       </c>
@@ -7650,8 +8256,12 @@
       <c r="O141" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:15">
+      <c r="P141" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16">
       <c r="A142" s="2" t="s">
         <v>144</v>
       </c>
@@ -7697,8 +8307,12 @@
       <c r="O142" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:15">
+      <c r="P142" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:16">
       <c r="A143" s="2" t="s">
         <v>145</v>
       </c>
@@ -7744,8 +8358,12 @@
       <c r="O143" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:15">
+      <c r="P143" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:16">
       <c r="A144" s="2" t="s">
         <v>146</v>
       </c>
@@ -7791,8 +8409,12 @@
       <c r="O144" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:15">
+      <c r="P144" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:16">
       <c r="A145" s="2" t="s">
         <v>147</v>
       </c>
@@ -7838,8 +8460,12 @@
       <c r="O145" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:15">
+      <c r="P145" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:16">
       <c r="A146" s="2" t="s">
         <v>148</v>
       </c>
@@ -7885,8 +8511,12 @@
       <c r="O146" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:15">
+      <c r="P146" s="1">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="147" spans="1:16">
       <c r="A147" s="2" t="s">
         <v>149</v>
       </c>
@@ -7932,8 +8562,12 @@
       <c r="O147" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:15">
+      <c r="P147" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16">
       <c r="A148" s="2" t="s">
         <v>150</v>
       </c>
@@ -7979,8 +8613,12 @@
       <c r="O148" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:15">
+      <c r="P148" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:16">
       <c r="A149" s="2" t="s">
         <v>151</v>
       </c>
@@ -8026,8 +8664,12 @@
       <c r="O149" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:15">
+      <c r="P149" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:16">
       <c r="A150" s="2" t="s">
         <v>152</v>
       </c>
@@ -8073,8 +8715,12 @@
       <c r="O150" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:15">
+      <c r="P150" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16">
       <c r="A151" s="2" t="s">
         <v>153</v>
       </c>
@@ -8120,8 +8766,12 @@
       <c r="O151" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:15">
+      <c r="P151" s="1">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16">
       <c r="A152" s="2" t="s">
         <v>154</v>
       </c>
@@ -8167,8 +8817,12 @@
       <c r="O152" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="1:15">
+      <c r="P152" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16">
       <c r="A153" s="2" t="s">
         <v>155</v>
       </c>
@@ -8214,8 +8868,12 @@
       <c r="O153" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:15">
+      <c r="P153" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16">
       <c r="A154" s="2" t="s">
         <v>156</v>
       </c>
@@ -8261,8 +8919,12 @@
       <c r="O154" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:15">
+      <c r="P154" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16">
       <c r="A155" s="2" t="s">
         <v>157</v>
       </c>
@@ -8308,8 +8970,12 @@
       <c r="O155" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="156" spans="1:15">
+      <c r="P155" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16">
       <c r="A156" s="2" t="s">
         <v>158</v>
       </c>
@@ -8355,8 +9021,12 @@
       <c r="O156" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:15">
+      <c r="P156" s="1">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:16">
       <c r="A157" s="2" t="s">
         <v>159</v>
       </c>
@@ -8402,8 +9072,12 @@
       <c r="O157" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="1:15">
+      <c r="P157" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:16">
       <c r="A158" s="2" t="s">
         <v>160</v>
       </c>
@@ -8449,8 +9123,12 @@
       <c r="O158" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="159" spans="1:15">
+      <c r="P158" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:16">
       <c r="A159" s="2" t="s">
         <v>161</v>
       </c>
@@ -8496,8 +9174,12 @@
       <c r="O159" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="160" spans="1:15">
+      <c r="P159" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:16">
       <c r="A160" s="2" t="s">
         <v>162</v>
       </c>
@@ -8543,8 +9225,12 @@
       <c r="O160" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="1:15">
+      <c r="P160" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:16">
       <c r="A161" s="2" t="s">
         <v>163</v>
       </c>
@@ -8590,8 +9276,12 @@
       <c r="O161" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="1:15">
+      <c r="P161" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:16">
       <c r="A162" s="2" t="s">
         <v>164</v>
       </c>
@@ -8637,8 +9327,12 @@
       <c r="O162" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="163" spans="1:15">
+      <c r="P162" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:16">
       <c r="A163" s="2" t="s">
         <v>165</v>
       </c>
@@ -8684,8 +9378,12 @@
       <c r="O163" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="164" spans="1:15">
+      <c r="P163" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:16">
       <c r="A164" s="2" t="s">
         <v>166</v>
       </c>
@@ -8731,8 +9429,12 @@
       <c r="O164" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:15">
+      <c r="P164" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:16">
       <c r="A165" s="2" t="s">
         <v>167</v>
       </c>
@@ -8778,8 +9480,12 @@
       <c r="O165" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="166" spans="1:15">
+      <c r="P165" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="1:16">
       <c r="A166" s="2" t="s">
         <v>168</v>
       </c>
@@ -8825,8 +9531,12 @@
       <c r="O166" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="1:15">
+      <c r="P166" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:16">
       <c r="A167" s="2" t="s">
         <v>169</v>
       </c>
@@ -8872,8 +9582,12 @@
       <c r="O167" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="168" spans="1:15">
+      <c r="P167" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:16">
       <c r="A168" s="2" t="s">
         <v>170</v>
       </c>
@@ -8919,8 +9633,12 @@
       <c r="O168" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="1:15">
+      <c r="P168" s="1">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:16">
       <c r="A169" s="2" t="s">
         <v>171</v>
       </c>
@@ -8966,8 +9684,12 @@
       <c r="O169" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="170" spans="1:15">
+      <c r="P169" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:16">
       <c r="A170" s="2" t="s">
         <v>172</v>
       </c>
@@ -9013,8 +9735,12 @@
       <c r="O170" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="171" spans="1:15">
+      <c r="P170" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:16">
       <c r="A171" s="2" t="s">
         <v>173</v>
       </c>
@@ -9060,8 +9786,12 @@
       <c r="O171" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="172" spans="1:15">
+      <c r="P171" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:16">
       <c r="A172" s="2" t="s">
         <v>174</v>
       </c>
@@ -9107,8 +9837,12 @@
       <c r="O172" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="173" spans="1:15">
+      <c r="P172" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:16">
       <c r="A173" s="2" t="s">
         <v>175</v>
       </c>
@@ -9154,8 +9888,12 @@
       <c r="O173" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="174" spans="1:15">
+      <c r="P173" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:16">
       <c r="A174" s="2" t="s">
         <v>176</v>
       </c>
@@ -9201,8 +9939,12 @@
       <c r="O174" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="175" spans="1:15">
+      <c r="P174" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:16">
       <c r="A175" s="2" t="s">
         <v>177</v>
       </c>
@@ -9248,8 +9990,12 @@
       <c r="O175" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="176" spans="1:15">
+      <c r="P175" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:16">
       <c r="A176" s="2" t="s">
         <v>178</v>
       </c>
@@ -9295,8 +10041,12 @@
       <c r="O176" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="177" spans="1:15">
+      <c r="P176" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:16">
       <c r="A177" s="2" t="s">
         <v>179</v>
       </c>
@@ -9342,8 +10092,12 @@
       <c r="O177" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="178" spans="1:15">
+      <c r="P177" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:16">
       <c r="A178" s="2" t="s">
         <v>180</v>
       </c>
@@ -9389,8 +10143,12 @@
       <c r="O178" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="179" spans="1:15">
+      <c r="P178" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:16">
       <c r="A179" s="2" t="s">
         <v>181</v>
       </c>
@@ -9436,8 +10194,12 @@
       <c r="O179" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="180" spans="1:15">
+      <c r="P179" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:16">
       <c r="A180" s="2" t="s">
         <v>182</v>
       </c>
@@ -9483,8 +10245,12 @@
       <c r="O180" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="181" spans="1:15">
+      <c r="P180" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:16">
       <c r="A181" s="2" t="s">
         <v>183</v>
       </c>
@@ -9530,8 +10296,12 @@
       <c r="O181" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="1:15">
+      <c r="P181" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:16">
       <c r="A182" s="2" t="s">
         <v>184</v>
       </c>
@@ -9577,8 +10347,12 @@
       <c r="O182" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="183" spans="1:15">
+      <c r="P182" s="1">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:16">
       <c r="A183" s="2" t="s">
         <v>185</v>
       </c>
@@ -9624,8 +10398,12 @@
       <c r="O183" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="184" spans="1:15">
+      <c r="P183" s="1">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="184" spans="1:16">
       <c r="A184" s="2" t="s">
         <v>186</v>
       </c>
@@ -9671,8 +10449,12 @@
       <c r="O184" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="185" spans="1:15">
+      <c r="P184" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:16">
       <c r="A185" s="2" t="s">
         <v>187</v>
       </c>
@@ -9718,8 +10500,12 @@
       <c r="O185" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="186" spans="1:15">
+      <c r="P185" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:16">
       <c r="A186" s="2" t="s">
         <v>188</v>
       </c>
@@ -9765,8 +10551,12 @@
       <c r="O186" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="187" spans="1:15">
+      <c r="P186" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:16">
       <c r="A187" s="2" t="s">
         <v>189</v>
       </c>
@@ -9812,8 +10602,12 @@
       <c r="O187" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="188" spans="1:15">
+      <c r="P187" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:16">
       <c r="A188" s="2" t="s">
         <v>190</v>
       </c>
@@ -9859,8 +10653,12 @@
       <c r="O188" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="189" spans="1:15">
+      <c r="P188" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:16">
       <c r="A189" s="2" t="s">
         <v>191</v>
       </c>
@@ -9906,8 +10704,12 @@
       <c r="O189" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="190" spans="1:15">
+      <c r="P189" s="1">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:16">
       <c r="A190" s="2" t="s">
         <v>192</v>
       </c>
@@ -9953,8 +10755,12 @@
       <c r="O190" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="191" spans="1:15">
+      <c r="P190" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:16">
       <c r="A191" s="2" t="s">
         <v>193</v>
       </c>
@@ -10000,8 +10806,12 @@
       <c r="O191" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="192" spans="1:15">
+      <c r="P191" s="1">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="192" spans="1:16">
       <c r="A192" s="2" t="s">
         <v>194</v>
       </c>
@@ -10047,8 +10857,12 @@
       <c r="O192" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="193" spans="1:15">
+      <c r="P192" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="193" spans="1:16">
       <c r="A193" s="2" t="s">
         <v>195</v>
       </c>
@@ -10094,8 +10908,12 @@
       <c r="O193" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="194" spans="1:15">
+      <c r="P193" s="1">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:16">
       <c r="A194" s="2" t="s">
         <v>196</v>
       </c>
@@ -10141,8 +10959,12 @@
       <c r="O194" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="195" spans="1:15">
+      <c r="P194" s="1">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:16">
       <c r="A195" s="2" t="s">
         <v>197</v>
       </c>
@@ -10188,8 +11010,12 @@
       <c r="O195" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="196" spans="1:15">
+      <c r="P195" s="1">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="196" spans="1:16">
       <c r="A196" s="2" t="s">
         <v>198</v>
       </c>
@@ -10235,8 +11061,12 @@
       <c r="O196" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="197" spans="1:15">
+      <c r="P196" s="1">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:16">
       <c r="A197" s="2" t="s">
         <v>199</v>
       </c>
@@ -10282,8 +11112,12 @@
       <c r="O197" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="198" spans="1:15">
+      <c r="P197" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="198" spans="1:16">
       <c r="A198" s="2" t="s">
         <v>200</v>
       </c>
@@ -10329,8 +11163,12 @@
       <c r="O198" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="199" spans="1:15">
+      <c r="P198" s="1">
+        <f t="shared" ref="P198:P222" si="3">SUM(B198:O198)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199" spans="1:16">
       <c r="A199" s="2" t="s">
         <v>201</v>
       </c>
@@ -10376,8 +11214,12 @@
       <c r="O199" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="200" spans="1:15">
+      <c r="P199" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:16">
       <c r="A200" s="2" t="s">
         <v>202</v>
       </c>
@@ -10423,8 +11265,12 @@
       <c r="O200" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="201" spans="1:15">
+      <c r="P200" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="201" spans="1:16">
       <c r="A201" s="2" t="s">
         <v>203</v>
       </c>
@@ -10470,8 +11316,12 @@
       <c r="O201" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="202" spans="1:15">
+      <c r="P201" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="202" spans="1:16">
       <c r="A202" s="2" t="s">
         <v>204</v>
       </c>
@@ -10517,8 +11367,12 @@
       <c r="O202" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="203" spans="1:15">
+      <c r="P202" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="203" spans="1:16">
       <c r="A203" s="2" t="s">
         <v>205</v>
       </c>
@@ -10564,8 +11418,12 @@
       <c r="O203" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="204" spans="1:15">
+      <c r="P203" s="1">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="204" spans="1:16">
       <c r="A204" s="2" t="s">
         <v>206</v>
       </c>
@@ -10611,8 +11469,12 @@
       <c r="O204" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="205" spans="1:15">
+      <c r="P204" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:16">
       <c r="A205" s="2" t="s">
         <v>207</v>
       </c>
@@ -10658,8 +11520,12 @@
       <c r="O205" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="206" spans="1:15">
+      <c r="P205" s="1">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="206" spans="1:16">
       <c r="A206" s="2" t="s">
         <v>208</v>
       </c>
@@ -10705,8 +11571,12 @@
       <c r="O206" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="207" spans="1:15">
+      <c r="P206" s="1">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="207" spans="1:16">
       <c r="A207" s="2" t="s">
         <v>209</v>
       </c>
@@ -10752,8 +11622,12 @@
       <c r="O207" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="208" spans="1:15">
+      <c r="P207" s="1">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="208" spans="1:16">
       <c r="A208" s="2" t="s">
         <v>210</v>
       </c>
@@ -10799,8 +11673,12 @@
       <c r="O208" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="209" spans="1:15">
+      <c r="P208" s="1">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="209" spans="1:16">
       <c r="A209" s="2" t="s">
         <v>211</v>
       </c>
@@ -10846,8 +11724,12 @@
       <c r="O209" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="210" spans="1:15">
+      <c r="P209" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:16">
       <c r="A210" s="2" t="s">
         <v>212</v>
       </c>
@@ -10893,8 +11775,12 @@
       <c r="O210" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="211" spans="1:15">
+      <c r="P210" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:16">
       <c r="A211" s="2" t="s">
         <v>213</v>
       </c>
@@ -10940,8 +11826,12 @@
       <c r="O211" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="212" spans="1:15">
+      <c r="P211" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:16">
       <c r="A212" s="2" t="s">
         <v>214</v>
       </c>
@@ -10987,8 +11877,12 @@
       <c r="O212" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="213" spans="1:15">
+      <c r="P212" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="213" spans="1:16">
       <c r="A213" s="2" t="s">
         <v>215</v>
       </c>
@@ -11034,8 +11928,12 @@
       <c r="O213" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="214" spans="1:15">
+      <c r="P213" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="214" spans="1:16">
       <c r="A214" s="2" t="s">
         <v>216</v>
       </c>
@@ -11081,8 +11979,12 @@
       <c r="O214" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="215" spans="1:15">
+      <c r="P214" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="215" spans="1:16">
       <c r="A215" s="2" t="s">
         <v>217</v>
       </c>
@@ -11128,8 +12030,12 @@
       <c r="O215" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="216" spans="1:15">
+      <c r="P215" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="216" spans="1:16">
       <c r="A216" s="2" t="s">
         <v>218</v>
       </c>
@@ -11175,8 +12081,12 @@
       <c r="O216" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="217" spans="1:15">
+      <c r="P216" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:16">
       <c r="A217" s="2" t="s">
         <v>219</v>
       </c>
@@ -11222,8 +12132,12 @@
       <c r="O217" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="218" spans="1:15">
+      <c r="P217" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:16">
       <c r="A218" s="2" t="s">
         <v>220</v>
       </c>
@@ -11269,8 +12183,12 @@
       <c r="O218" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="219" spans="1:15">
+      <c r="P218" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="219" spans="1:16">
       <c r="A219" s="2" t="s">
         <v>221</v>
       </c>
@@ -11316,8 +12234,12 @@
       <c r="O219" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="220" spans="1:15">
+      <c r="P219" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="220" spans="1:16">
       <c r="A220" s="2" t="s">
         <v>222</v>
       </c>
@@ -11363,8 +12285,12 @@
       <c r="O220" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="221" spans="1:15">
+      <c r="P220" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:16">
       <c r="A221" s="2" t="s">
         <v>223</v>
       </c>
@@ -11410,8 +12336,12 @@
       <c r="O221" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="222" spans="1:15">
+      <c r="P221" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:16" ht="15" thickBot="1">
       <c r="A222" s="1" t="s">
         <v>224</v>
       </c>
@@ -11457,63 +12387,226 @@
       <c r="O222" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="223" spans="1:15">
-      <c r="B223">
-        <f t="shared" ref="B223:O223" si="0">SUM(B4:B222)</f>
+      <c r="P222" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:16" ht="15" thickBot="1">
+      <c r="A223" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B223" s="1">
+        <f t="shared" ref="B223:O223" si="4">SUM(B4:B222)</f>
         <v>111</v>
       </c>
-      <c r="C223">
-        <f t="shared" si="0"/>
+      <c r="C223" s="1">
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
-      <c r="D223">
-        <f t="shared" si="0"/>
+      <c r="D223" s="1">
+        <f t="shared" si="4"/>
         <v>106</v>
       </c>
-      <c r="E223">
-        <f t="shared" si="0"/>
+      <c r="E223" s="1">
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
-      <c r="F223">
-        <f t="shared" si="0"/>
+      <c r="F223" s="1">
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
-      <c r="G223">
-        <f t="shared" si="0"/>
-        <v>103</v>
-      </c>
-      <c r="H223">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I223">
-        <f t="shared" si="0"/>
+      <c r="G223" s="1">
+        <f t="shared" si="4"/>
+        <v>102</v>
+      </c>
+      <c r="H223" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I223" s="1">
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="J223">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K223">
-        <f t="shared" si="0"/>
+      <c r="J223" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K223" s="1">
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="L223">
-        <f t="shared" si="0"/>
+      <c r="L223" s="1">
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
-      <c r="M223">
-        <f t="shared" si="0"/>
+      <c r="M223" s="1">
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
-      <c r="N223">
-        <f t="shared" si="0"/>
+      <c r="N223" s="1">
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="O223">
-        <f t="shared" si="0"/>
+      <c r="O223" s="4">
+        <f t="shared" si="4"/>
         <v>7</v>
+      </c>
+      <c r="P223" s="7"/>
+    </row>
+    <row r="225" spans="1:2">
+      <c r="A225" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2">
+      <c r="A226" s="1">
+        <f>AVERAGE(P4:P222)</f>
+        <v>2.3607305936073057</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2">
+      <c r="A227" s="8"/>
+    </row>
+    <row r="228" spans="1:2">
+      <c r="A228" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B228" s="1"/>
+    </row>
+    <row r="229" spans="1:2">
+      <c r="A229" s="5">
+        <v>0</v>
+      </c>
+      <c r="B229" s="1">
+        <f>COUNTIF(P4:P222, 0)</f>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2">
+      <c r="A230" s="1">
+        <v>1</v>
+      </c>
+      <c r="B230" s="1">
+        <f>COUNTIF(P4:P222, 1)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2">
+      <c r="A231" s="1">
+        <v>2</v>
+      </c>
+      <c r="B231" s="1">
+        <f>COUNTIF(P4:P222, 2)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2">
+      <c r="A232" s="1">
+        <v>3</v>
+      </c>
+      <c r="B232" s="1">
+        <f>COUNTIF(P4:P222, 3)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2">
+      <c r="A233" s="1">
+        <v>4</v>
+      </c>
+      <c r="B233" s="1">
+        <f>COUNTIF(P4:P222, 4)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2">
+      <c r="A234" s="1">
+        <v>5</v>
+      </c>
+      <c r="B234" s="1">
+        <f>COUNTIF(P4:P222, 5)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2">
+      <c r="A235" s="1">
+        <v>6</v>
+      </c>
+      <c r="B235" s="1">
+        <f>COUNTIF(P4:P222, 6)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2">
+      <c r="A236" s="1">
+        <v>7</v>
+      </c>
+      <c r="B236" s="1">
+        <f>COUNTIF(P4:P222, 7)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2">
+      <c r="A237" s="1">
+        <v>8</v>
+      </c>
+      <c r="B237" s="1">
+        <f>COUNTIF(P4:P222, 8)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2">
+      <c r="A238" s="1">
+        <v>9</v>
+      </c>
+      <c r="B238" s="1">
+        <f>COUNTIF(P4:P222, 9)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2">
+      <c r="A239" s="1">
+        <v>10</v>
+      </c>
+      <c r="B239" s="1">
+        <f>COUNTIF(P4:P222, 10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2">
+      <c r="A240" s="1">
+        <v>11</v>
+      </c>
+      <c r="B240" s="1">
+        <f>COUNTIF(P4:P222, 11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2">
+      <c r="A241" s="1">
+        <v>12</v>
+      </c>
+      <c r="B241" s="1">
+        <f>COUNTIF(P4:P222, 12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2">
+      <c r="A242" s="1">
+        <v>13</v>
+      </c>
+      <c r="B242" s="1">
+        <f>COUNTIF(P4:P222, 13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2">
+      <c r="A243" s="1">
+        <v>14</v>
+      </c>
+      <c r="B243" s="1">
+        <f>COUNTIF(P4:P222, 14)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
performance.py is the script to compare CLIP and EasyOCR. Folder SigLIP added (not working on my computer, but may be useful at some point)
</commit_message>
<xml_diff>
--- a/labellisation.xlsx
+++ b/labellisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nizon\Documents\Perso\Cours\Cours 4A\The AI Lifecycle\App-For-People-With-Restricted-Diet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DF2159-5E43-4E0B-B56D-CA7D722754EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1575E2C-AA65-49F5-AA09-6BC37BD47F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1149,8 +1149,8 @@
   <dimension ref="A1:P243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A214" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L223" sqref="L223"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -1241,7 +1241,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="P4" s="1">
         <f>SUM(B4:O4)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -12395,59 +12395,59 @@
         <v>233</v>
       </c>
       <c r="B223" s="1">
-        <f>SUM(B4:B222)</f>
+        <f t="shared" ref="B223:O223" si="4">SUM(B4:B222)</f>
         <v>111</v>
       </c>
       <c r="C223" s="1">
-        <f>SUM(C4:C222)</f>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="D223" s="1">
-        <f>SUM(D4:D222)</f>
+        <f t="shared" si="4"/>
         <v>106</v>
       </c>
       <c r="E223" s="1">
-        <f>SUM(E4:E222)</f>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="F223" s="1">
-        <f>SUM(F4:F222)</f>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="G223" s="1">
-        <f>SUM(G4:G222)</f>
-        <v>102</v>
+        <f t="shared" si="4"/>
+        <v>103</v>
       </c>
       <c r="H223" s="1">
-        <f>SUM(H4:H222)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I223" s="1">
-        <f>SUM(I4:I222)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="J223" s="1">
-        <f>SUM(J4:J222)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K223" s="1">
-        <f>SUM(K4:K222)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="L223" s="1">
-        <f>SUM(L4:L222)</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="M223" s="1">
-        <f>SUM(M4:M222)</f>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="N223" s="1">
-        <f>SUM(N4:N222)</f>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="O223" s="3">
-        <f>SUM(O4:O222)</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="P223" s="5"/>
@@ -12460,7 +12460,7 @@
     <row r="226" spans="1:2">
       <c r="A226" s="1">
         <f>AVERAGE(P4:P222)</f>
-        <v>2.3607305936073057</v>
+        <v>2.365296803652968</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -12520,7 +12520,7 @@
       </c>
       <c r="B234" s="1">
         <f>COUNTIF(P4:P222, 5)</f>
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="235" spans="1:2">
@@ -12529,7 +12529,7 @@
       </c>
       <c r="B235" s="1">
         <f>COUNTIF(P4:P222, 6)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="236" spans="1:2">

</xml_diff>